<commit_message>
create folder named after todays date, create excel files based off of template and named after customer
</commit_message>
<xml_diff>
--- a/customerqueue/tgtr1.xlsx
+++ b/customerqueue/tgtr1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\customerqueue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC62487-C8B8-4AFA-9240-BFBC3E1BBDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A002A0-6100-4D70-AD82-849FCF9B4911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3132" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rdt1.xlsx" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -565,7 +565,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -948,7 +948,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1060,7 +1060,7 @@
         <v>45094</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>

</xml_diff>